<commit_message>
Updated with 04/05/2022 data
</commit_message>
<xml_diff>
--- a/data/octanol_30pct_avoidance_ALLDATA.xlsx
+++ b/data/octanol_30pct_avoidance_ALLDATA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tiabrown/Documents/git/cest-2.1-Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F1C1D4-99A5-A044-A77C-04E99D4C02F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F54821-55AE-F946-8F6D-4E2AB496A302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2007" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2375" uniqueCount="17">
   <si>
     <t>genotype</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>MD</t>
+  </si>
+  <si>
+    <t>tbh-1</t>
   </si>
 </sst>
 </file>
@@ -926,11 +929,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G501"/>
+  <dimension ref="A1:G593"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A476" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H492" sqref="H492"/>
+      <pane ySplit="1" topLeftCell="A573" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J586" sqref="J586"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10960,6 +10963,1846 @@
         <v>44645</v>
       </c>
     </row>
+    <row r="502" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A502" t="s">
+        <v>16</v>
+      </c>
+      <c r="B502" t="s">
+        <v>13</v>
+      </c>
+      <c r="C502" t="s">
+        <v>6</v>
+      </c>
+      <c r="D502">
+        <v>4.75</v>
+      </c>
+      <c r="E502" t="s">
+        <v>9</v>
+      </c>
+      <c r="F502" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="503" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A503" t="s">
+        <v>16</v>
+      </c>
+      <c r="B503" t="s">
+        <v>13</v>
+      </c>
+      <c r="C503" t="s">
+        <v>6</v>
+      </c>
+      <c r="D503">
+        <v>6.75</v>
+      </c>
+      <c r="E503" t="s">
+        <v>9</v>
+      </c>
+      <c r="F503" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="504" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A504" t="s">
+        <v>16</v>
+      </c>
+      <c r="B504" t="s">
+        <v>13</v>
+      </c>
+      <c r="C504" t="s">
+        <v>6</v>
+      </c>
+      <c r="D504">
+        <v>9.23</v>
+      </c>
+      <c r="E504" t="s">
+        <v>9</v>
+      </c>
+      <c r="F504" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="505" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A505" t="s">
+        <v>16</v>
+      </c>
+      <c r="B505" t="s">
+        <v>13</v>
+      </c>
+      <c r="C505" t="s">
+        <v>6</v>
+      </c>
+      <c r="D505">
+        <v>7.44</v>
+      </c>
+      <c r="E505" t="s">
+        <v>9</v>
+      </c>
+      <c r="F505" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="506" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A506" t="s">
+        <v>16</v>
+      </c>
+      <c r="B506" t="s">
+        <v>13</v>
+      </c>
+      <c r="C506" t="s">
+        <v>6</v>
+      </c>
+      <c r="D506">
+        <v>5.4</v>
+      </c>
+      <c r="E506" t="s">
+        <v>9</v>
+      </c>
+      <c r="F506" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="507" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A507" t="s">
+        <v>16</v>
+      </c>
+      <c r="B507" t="s">
+        <v>13</v>
+      </c>
+      <c r="C507" t="s">
+        <v>6</v>
+      </c>
+      <c r="D507">
+        <v>6.3</v>
+      </c>
+      <c r="E507" t="s">
+        <v>9</v>
+      </c>
+      <c r="F507" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="508" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A508" t="s">
+        <v>16</v>
+      </c>
+      <c r="B508" t="s">
+        <v>13</v>
+      </c>
+      <c r="C508" t="s">
+        <v>6</v>
+      </c>
+      <c r="D508">
+        <v>7.94</v>
+      </c>
+      <c r="E508" t="s">
+        <v>9</v>
+      </c>
+      <c r="F508" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="509" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A509" t="s">
+        <v>16</v>
+      </c>
+      <c r="B509" t="s">
+        <v>13</v>
+      </c>
+      <c r="C509" t="s">
+        <v>6</v>
+      </c>
+      <c r="D509">
+        <v>3.23</v>
+      </c>
+      <c r="E509" t="s">
+        <v>9</v>
+      </c>
+      <c r="F509" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="510" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A510" t="s">
+        <v>16</v>
+      </c>
+      <c r="B510" t="s">
+        <v>13</v>
+      </c>
+      <c r="C510" t="s">
+        <v>6</v>
+      </c>
+      <c r="D510">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="E510" t="s">
+        <v>9</v>
+      </c>
+      <c r="F510" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="511" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A511" t="s">
+        <v>16</v>
+      </c>
+      <c r="B511" t="s">
+        <v>13</v>
+      </c>
+      <c r="C511" t="s">
+        <v>6</v>
+      </c>
+      <c r="D511">
+        <v>5.23</v>
+      </c>
+      <c r="E511" t="s">
+        <v>9</v>
+      </c>
+      <c r="F511" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="512" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A512" t="s">
+        <v>16</v>
+      </c>
+      <c r="B512" t="s">
+        <v>13</v>
+      </c>
+      <c r="C512" t="s">
+        <v>6</v>
+      </c>
+      <c r="D512">
+        <v>2.82</v>
+      </c>
+      <c r="E512" t="s">
+        <v>9</v>
+      </c>
+      <c r="F512" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="513" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A513" t="s">
+        <v>16</v>
+      </c>
+      <c r="B513" t="s">
+        <v>13</v>
+      </c>
+      <c r="C513" t="s">
+        <v>6</v>
+      </c>
+      <c r="D513">
+        <v>4.4400000000000004</v>
+      </c>
+      <c r="E513" t="s">
+        <v>9</v>
+      </c>
+      <c r="F513" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="514" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A514" t="s">
+        <v>16</v>
+      </c>
+      <c r="B514" t="s">
+        <v>13</v>
+      </c>
+      <c r="C514" t="s">
+        <v>6</v>
+      </c>
+      <c r="D514">
+        <v>3.19</v>
+      </c>
+      <c r="E514" t="s">
+        <v>9</v>
+      </c>
+      <c r="F514" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="515" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A515" t="s">
+        <v>16</v>
+      </c>
+      <c r="B515" t="s">
+        <v>13</v>
+      </c>
+      <c r="C515" t="s">
+        <v>6</v>
+      </c>
+      <c r="D515">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="E515" t="s">
+        <v>9</v>
+      </c>
+      <c r="F515" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="516" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A516" t="s">
+        <v>16</v>
+      </c>
+      <c r="B516" t="s">
+        <v>13</v>
+      </c>
+      <c r="C516" t="s">
+        <v>6</v>
+      </c>
+      <c r="D516">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="E516" t="s">
+        <v>9</v>
+      </c>
+      <c r="F516" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="517" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A517" t="s">
+        <v>16</v>
+      </c>
+      <c r="B517" t="s">
+        <v>13</v>
+      </c>
+      <c r="C517" t="s">
+        <v>6</v>
+      </c>
+      <c r="D517">
+        <v>6.59</v>
+      </c>
+      <c r="E517" t="s">
+        <v>9</v>
+      </c>
+      <c r="F517" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="518" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A518" t="s">
+        <v>8</v>
+      </c>
+      <c r="B518" t="s">
+        <v>13</v>
+      </c>
+      <c r="C518" t="s">
+        <v>6</v>
+      </c>
+      <c r="D518">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="E518" t="s">
+        <v>9</v>
+      </c>
+      <c r="F518" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="519" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A519" t="s">
+        <v>8</v>
+      </c>
+      <c r="B519" t="s">
+        <v>13</v>
+      </c>
+      <c r="C519" t="s">
+        <v>6</v>
+      </c>
+      <c r="D519">
+        <v>3.84</v>
+      </c>
+      <c r="E519" t="s">
+        <v>9</v>
+      </c>
+      <c r="F519" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="520" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A520" t="s">
+        <v>8</v>
+      </c>
+      <c r="B520" t="s">
+        <v>13</v>
+      </c>
+      <c r="C520" t="s">
+        <v>6</v>
+      </c>
+      <c r="D520">
+        <v>2.64</v>
+      </c>
+      <c r="E520" t="s">
+        <v>9</v>
+      </c>
+      <c r="F520" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="521" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A521" t="s">
+        <v>8</v>
+      </c>
+      <c r="B521" t="s">
+        <v>13</v>
+      </c>
+      <c r="C521" t="s">
+        <v>6</v>
+      </c>
+      <c r="D521">
+        <v>3.35</v>
+      </c>
+      <c r="E521" t="s">
+        <v>9</v>
+      </c>
+      <c r="F521" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="522" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A522" t="s">
+        <v>8</v>
+      </c>
+      <c r="B522" t="s">
+        <v>13</v>
+      </c>
+      <c r="C522" t="s">
+        <v>6</v>
+      </c>
+      <c r="D522">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E522" t="s">
+        <v>9</v>
+      </c>
+      <c r="F522" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="523" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A523" t="s">
+        <v>8</v>
+      </c>
+      <c r="B523" t="s">
+        <v>13</v>
+      </c>
+      <c r="C523" t="s">
+        <v>6</v>
+      </c>
+      <c r="D523">
+        <v>3.54</v>
+      </c>
+      <c r="E523" t="s">
+        <v>9</v>
+      </c>
+      <c r="F523" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="524" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A524" t="s">
+        <v>8</v>
+      </c>
+      <c r="B524" t="s">
+        <v>13</v>
+      </c>
+      <c r="C524" t="s">
+        <v>6</v>
+      </c>
+      <c r="D524">
+        <v>3.06</v>
+      </c>
+      <c r="E524" t="s">
+        <v>9</v>
+      </c>
+      <c r="F524" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="525" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A525" t="s">
+        <v>8</v>
+      </c>
+      <c r="B525" t="s">
+        <v>13</v>
+      </c>
+      <c r="C525" t="s">
+        <v>6</v>
+      </c>
+      <c r="D525">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="E525" t="s">
+        <v>9</v>
+      </c>
+      <c r="F525" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="526" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A526" t="s">
+        <v>8</v>
+      </c>
+      <c r="B526" t="s">
+        <v>13</v>
+      </c>
+      <c r="C526" t="s">
+        <v>6</v>
+      </c>
+      <c r="D526">
+        <v>4.25</v>
+      </c>
+      <c r="E526" t="s">
+        <v>9</v>
+      </c>
+      <c r="F526" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="527" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A527" t="s">
+        <v>8</v>
+      </c>
+      <c r="B527" t="s">
+        <v>13</v>
+      </c>
+      <c r="C527" t="s">
+        <v>6</v>
+      </c>
+      <c r="D527">
+        <v>5.88</v>
+      </c>
+      <c r="E527" t="s">
+        <v>9</v>
+      </c>
+      <c r="F527" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="528" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A528" t="s">
+        <v>8</v>
+      </c>
+      <c r="B528" t="s">
+        <v>13</v>
+      </c>
+      <c r="C528" t="s">
+        <v>6</v>
+      </c>
+      <c r="D528">
+        <v>3.95</v>
+      </c>
+      <c r="E528" t="s">
+        <v>9</v>
+      </c>
+      <c r="F528" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="529" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A529" t="s">
+        <v>8</v>
+      </c>
+      <c r="B529" t="s">
+        <v>13</v>
+      </c>
+      <c r="C529" t="s">
+        <v>6</v>
+      </c>
+      <c r="D529">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="E529" t="s">
+        <v>9</v>
+      </c>
+      <c r="F529" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="530" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A530" t="s">
+        <v>8</v>
+      </c>
+      <c r="B530" t="s">
+        <v>13</v>
+      </c>
+      <c r="C530" t="s">
+        <v>6</v>
+      </c>
+      <c r="D530">
+        <v>4.5</v>
+      </c>
+      <c r="E530" t="s">
+        <v>9</v>
+      </c>
+      <c r="F530" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="531" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A531" t="s">
+        <v>8</v>
+      </c>
+      <c r="B531" t="s">
+        <v>13</v>
+      </c>
+      <c r="C531" t="s">
+        <v>6</v>
+      </c>
+      <c r="D531">
+        <v>4.38</v>
+      </c>
+      <c r="E531" t="s">
+        <v>9</v>
+      </c>
+      <c r="F531" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="532" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A532" t="s">
+        <v>8</v>
+      </c>
+      <c r="B532" t="s">
+        <v>13</v>
+      </c>
+      <c r="C532" t="s">
+        <v>6</v>
+      </c>
+      <c r="D532">
+        <v>5.55</v>
+      </c>
+      <c r="E532" t="s">
+        <v>9</v>
+      </c>
+      <c r="F532" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="533" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A533" t="s">
+        <v>8</v>
+      </c>
+      <c r="B533" t="s">
+        <v>13</v>
+      </c>
+      <c r="C533" t="s">
+        <v>6</v>
+      </c>
+      <c r="D533">
+        <v>3.26</v>
+      </c>
+      <c r="E533" t="s">
+        <v>9</v>
+      </c>
+      <c r="F533" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="534" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A534" t="s">
+        <v>5</v>
+      </c>
+      <c r="B534" t="s">
+        <v>13</v>
+      </c>
+      <c r="C534" t="s">
+        <v>6</v>
+      </c>
+      <c r="D534">
+        <v>12.82</v>
+      </c>
+      <c r="E534" t="s">
+        <v>9</v>
+      </c>
+      <c r="F534" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="535" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A535" t="s">
+        <v>5</v>
+      </c>
+      <c r="B535" t="s">
+        <v>13</v>
+      </c>
+      <c r="C535" t="s">
+        <v>6</v>
+      </c>
+      <c r="D535">
+        <v>6.16</v>
+      </c>
+      <c r="E535" t="s">
+        <v>9</v>
+      </c>
+      <c r="F535" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="536" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A536" t="s">
+        <v>5</v>
+      </c>
+      <c r="B536" t="s">
+        <v>13</v>
+      </c>
+      <c r="C536" t="s">
+        <v>6</v>
+      </c>
+      <c r="D536">
+        <v>6.89</v>
+      </c>
+      <c r="E536" t="s">
+        <v>9</v>
+      </c>
+      <c r="F536" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="537" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A537" t="s">
+        <v>5</v>
+      </c>
+      <c r="B537" t="s">
+        <v>13</v>
+      </c>
+      <c r="C537" t="s">
+        <v>6</v>
+      </c>
+      <c r="D537">
+        <v>8.56</v>
+      </c>
+      <c r="E537" t="s">
+        <v>9</v>
+      </c>
+      <c r="F537" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="538" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A538" t="s">
+        <v>5</v>
+      </c>
+      <c r="B538" t="s">
+        <v>13</v>
+      </c>
+      <c r="C538" t="s">
+        <v>6</v>
+      </c>
+      <c r="D538">
+        <v>4.26</v>
+      </c>
+      <c r="E538" t="s">
+        <v>9</v>
+      </c>
+      <c r="F538" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="539" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A539" t="s">
+        <v>5</v>
+      </c>
+      <c r="B539" t="s">
+        <v>13</v>
+      </c>
+      <c r="C539" t="s">
+        <v>6</v>
+      </c>
+      <c r="D539">
+        <v>11.92</v>
+      </c>
+      <c r="E539" t="s">
+        <v>9</v>
+      </c>
+      <c r="F539" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="540" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A540" t="s">
+        <v>5</v>
+      </c>
+      <c r="B540" t="s">
+        <v>13</v>
+      </c>
+      <c r="C540" t="s">
+        <v>6</v>
+      </c>
+      <c r="D540">
+        <v>7.25</v>
+      </c>
+      <c r="E540" t="s">
+        <v>9</v>
+      </c>
+      <c r="F540" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="541" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A541" t="s">
+        <v>5</v>
+      </c>
+      <c r="B541" t="s">
+        <v>13</v>
+      </c>
+      <c r="C541" t="s">
+        <v>6</v>
+      </c>
+      <c r="D541">
+        <v>5.26</v>
+      </c>
+      <c r="E541" t="s">
+        <v>9</v>
+      </c>
+      <c r="F541" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="542" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A542" t="s">
+        <v>5</v>
+      </c>
+      <c r="B542" t="s">
+        <v>13</v>
+      </c>
+      <c r="C542" t="s">
+        <v>6</v>
+      </c>
+      <c r="D542">
+        <v>6.25</v>
+      </c>
+      <c r="E542" t="s">
+        <v>9</v>
+      </c>
+      <c r="F542" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="543" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A543" t="s">
+        <v>5</v>
+      </c>
+      <c r="B543" t="s">
+        <v>13</v>
+      </c>
+      <c r="C543" t="s">
+        <v>6</v>
+      </c>
+      <c r="D543">
+        <v>9.15</v>
+      </c>
+      <c r="E543" t="s">
+        <v>9</v>
+      </c>
+      <c r="F543" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="544" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A544" t="s">
+        <v>5</v>
+      </c>
+      <c r="B544" t="s">
+        <v>13</v>
+      </c>
+      <c r="C544" t="s">
+        <v>6</v>
+      </c>
+      <c r="D544">
+        <v>14.08</v>
+      </c>
+      <c r="E544" t="s">
+        <v>9</v>
+      </c>
+      <c r="F544" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="545" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A545" t="s">
+        <v>5</v>
+      </c>
+      <c r="B545" t="s">
+        <v>13</v>
+      </c>
+      <c r="C545" t="s">
+        <v>6</v>
+      </c>
+      <c r="D545">
+        <v>11.96</v>
+      </c>
+      <c r="E545" t="s">
+        <v>9</v>
+      </c>
+      <c r="F545" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="546" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A546" t="s">
+        <v>5</v>
+      </c>
+      <c r="B546" t="s">
+        <v>13</v>
+      </c>
+      <c r="C546" t="s">
+        <v>6</v>
+      </c>
+      <c r="D546">
+        <v>7.59</v>
+      </c>
+      <c r="E546" t="s">
+        <v>9</v>
+      </c>
+      <c r="F546" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="547" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A547" t="s">
+        <v>5</v>
+      </c>
+      <c r="B547" t="s">
+        <v>13</v>
+      </c>
+      <c r="C547" t="s">
+        <v>6</v>
+      </c>
+      <c r="D547">
+        <v>8.73</v>
+      </c>
+      <c r="E547" t="s">
+        <v>9</v>
+      </c>
+      <c r="F547" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="548" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A548" t="s">
+        <v>5</v>
+      </c>
+      <c r="B548" t="s">
+        <v>13</v>
+      </c>
+      <c r="C548" t="s">
+        <v>6</v>
+      </c>
+      <c r="D548">
+        <v>7.7</v>
+      </c>
+      <c r="E548" t="s">
+        <v>9</v>
+      </c>
+      <c r="F548" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="549" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A549" t="s">
+        <v>5</v>
+      </c>
+      <c r="B549" t="s">
+        <v>13</v>
+      </c>
+      <c r="C549" t="s">
+        <v>6</v>
+      </c>
+      <c r="D549">
+        <v>5.79</v>
+      </c>
+      <c r="E549" t="s">
+        <v>9</v>
+      </c>
+      <c r="F549" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="550" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A550" t="s">
+        <v>5</v>
+      </c>
+      <c r="B550" t="s">
+        <v>13</v>
+      </c>
+      <c r="C550" t="s">
+        <v>6</v>
+      </c>
+      <c r="D550">
+        <v>15.47</v>
+      </c>
+      <c r="E550" t="s">
+        <v>9</v>
+      </c>
+      <c r="F550" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="551" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A551" t="s">
+        <v>5</v>
+      </c>
+      <c r="B551" t="s">
+        <v>13</v>
+      </c>
+      <c r="C551" t="s">
+        <v>6</v>
+      </c>
+      <c r="D551">
+        <v>4.97</v>
+      </c>
+      <c r="E551" t="s">
+        <v>9</v>
+      </c>
+      <c r="F551" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="552" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A552" t="s">
+        <v>5</v>
+      </c>
+      <c r="B552" t="s">
+        <v>13</v>
+      </c>
+      <c r="C552" t="s">
+        <v>6</v>
+      </c>
+      <c r="D552">
+        <v>5.76</v>
+      </c>
+      <c r="E552" t="s">
+        <v>9</v>
+      </c>
+      <c r="F552" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="553" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A553" t="s">
+        <v>16</v>
+      </c>
+      <c r="B553" t="s">
+        <v>13</v>
+      </c>
+      <c r="C553" t="s">
+        <v>6</v>
+      </c>
+      <c r="D553">
+        <v>6.48</v>
+      </c>
+      <c r="E553" t="s">
+        <v>15</v>
+      </c>
+      <c r="F553" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="554" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A554" t="s">
+        <v>16</v>
+      </c>
+      <c r="B554" t="s">
+        <v>13</v>
+      </c>
+      <c r="C554" t="s">
+        <v>6</v>
+      </c>
+      <c r="D554">
+        <v>4.53</v>
+      </c>
+      <c r="E554" t="s">
+        <v>15</v>
+      </c>
+      <c r="F554" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="555" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A555" t="s">
+        <v>16</v>
+      </c>
+      <c r="B555" t="s">
+        <v>13</v>
+      </c>
+      <c r="C555" t="s">
+        <v>6</v>
+      </c>
+      <c r="D555">
+        <v>10.19</v>
+      </c>
+      <c r="E555" t="s">
+        <v>15</v>
+      </c>
+      <c r="F555" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="556" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A556" t="s">
+        <v>16</v>
+      </c>
+      <c r="B556" t="s">
+        <v>13</v>
+      </c>
+      <c r="C556" t="s">
+        <v>6</v>
+      </c>
+      <c r="D556">
+        <v>1.66</v>
+      </c>
+      <c r="E556" t="s">
+        <v>15</v>
+      </c>
+      <c r="F556" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="557" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A557" t="s">
+        <v>16</v>
+      </c>
+      <c r="B557" t="s">
+        <v>13</v>
+      </c>
+      <c r="C557" t="s">
+        <v>6</v>
+      </c>
+      <c r="D557">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E557" t="s">
+        <v>15</v>
+      </c>
+      <c r="F557" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="558" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A558" t="s">
+        <v>16</v>
+      </c>
+      <c r="B558" t="s">
+        <v>13</v>
+      </c>
+      <c r="C558" t="s">
+        <v>6</v>
+      </c>
+      <c r="D558">
+        <v>4.88</v>
+      </c>
+      <c r="E558" t="s">
+        <v>15</v>
+      </c>
+      <c r="F558" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="559" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A559" t="s">
+        <v>16</v>
+      </c>
+      <c r="B559" t="s">
+        <v>13</v>
+      </c>
+      <c r="C559" t="s">
+        <v>6</v>
+      </c>
+      <c r="D559">
+        <v>5.21</v>
+      </c>
+      <c r="E559" t="s">
+        <v>15</v>
+      </c>
+      <c r="F559" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="560" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A560" t="s">
+        <v>16</v>
+      </c>
+      <c r="B560" t="s">
+        <v>13</v>
+      </c>
+      <c r="C560" t="s">
+        <v>6</v>
+      </c>
+      <c r="D560">
+        <v>8.14</v>
+      </c>
+      <c r="E560" t="s">
+        <v>15</v>
+      </c>
+      <c r="F560" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="561" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A561" t="s">
+        <v>16</v>
+      </c>
+      <c r="B561" t="s">
+        <v>13</v>
+      </c>
+      <c r="C561" t="s">
+        <v>6</v>
+      </c>
+      <c r="D561">
+        <v>2.89</v>
+      </c>
+      <c r="E561" t="s">
+        <v>15</v>
+      </c>
+      <c r="F561" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="562" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A562" t="s">
+        <v>16</v>
+      </c>
+      <c r="B562" t="s">
+        <v>13</v>
+      </c>
+      <c r="C562" t="s">
+        <v>6</v>
+      </c>
+      <c r="D562">
+        <v>5.84</v>
+      </c>
+      <c r="E562" t="s">
+        <v>15</v>
+      </c>
+      <c r="F562" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="563" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A563" t="s">
+        <v>16</v>
+      </c>
+      <c r="B563" t="s">
+        <v>13</v>
+      </c>
+      <c r="C563" t="s">
+        <v>6</v>
+      </c>
+      <c r="D563">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="E563" t="s">
+        <v>15</v>
+      </c>
+      <c r="F563" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="564" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A564" t="s">
+        <v>16</v>
+      </c>
+      <c r="B564" t="s">
+        <v>13</v>
+      </c>
+      <c r="C564" t="s">
+        <v>6</v>
+      </c>
+      <c r="D564">
+        <v>4.91</v>
+      </c>
+      <c r="E564" t="s">
+        <v>15</v>
+      </c>
+      <c r="F564" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="565" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A565" t="s">
+        <v>16</v>
+      </c>
+      <c r="B565" t="s">
+        <v>13</v>
+      </c>
+      <c r="C565" t="s">
+        <v>6</v>
+      </c>
+      <c r="D565">
+        <v>5.01</v>
+      </c>
+      <c r="E565" t="s">
+        <v>15</v>
+      </c>
+      <c r="F565" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="566" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A566" t="s">
+        <v>16</v>
+      </c>
+      <c r="B566" t="s">
+        <v>13</v>
+      </c>
+      <c r="C566" t="s">
+        <v>6</v>
+      </c>
+      <c r="D566">
+        <v>5.34</v>
+      </c>
+      <c r="E566" t="s">
+        <v>15</v>
+      </c>
+      <c r="F566" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="567" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A567" t="s">
+        <v>8</v>
+      </c>
+      <c r="B567" t="s">
+        <v>13</v>
+      </c>
+      <c r="C567" t="s">
+        <v>6</v>
+      </c>
+      <c r="D567">
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="E567" t="s">
+        <v>15</v>
+      </c>
+      <c r="F567" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="568" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A568" t="s">
+        <v>8</v>
+      </c>
+      <c r="B568" t="s">
+        <v>13</v>
+      </c>
+      <c r="C568" t="s">
+        <v>6</v>
+      </c>
+      <c r="D568">
+        <v>2.94</v>
+      </c>
+      <c r="E568" t="s">
+        <v>15</v>
+      </c>
+      <c r="F568" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="569" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A569" t="s">
+        <v>8</v>
+      </c>
+      <c r="B569" t="s">
+        <v>13</v>
+      </c>
+      <c r="C569" t="s">
+        <v>6</v>
+      </c>
+      <c r="D569">
+        <v>2.58</v>
+      </c>
+      <c r="E569" t="s">
+        <v>15</v>
+      </c>
+      <c r="F569" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="570" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A570" t="s">
+        <v>8</v>
+      </c>
+      <c r="B570" t="s">
+        <v>13</v>
+      </c>
+      <c r="C570" t="s">
+        <v>6</v>
+      </c>
+      <c r="D570">
+        <v>6.266</v>
+      </c>
+      <c r="E570" t="s">
+        <v>15</v>
+      </c>
+      <c r="F570" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="571" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A571" t="s">
+        <v>8</v>
+      </c>
+      <c r="B571" t="s">
+        <v>13</v>
+      </c>
+      <c r="C571" t="s">
+        <v>6</v>
+      </c>
+      <c r="D571">
+        <v>3.91</v>
+      </c>
+      <c r="E571" t="s">
+        <v>15</v>
+      </c>
+      <c r="F571" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="572" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A572" t="s">
+        <v>8</v>
+      </c>
+      <c r="B572" t="s">
+        <v>13</v>
+      </c>
+      <c r="C572" t="s">
+        <v>6</v>
+      </c>
+      <c r="D572">
+        <v>10.43</v>
+      </c>
+      <c r="E572" t="s">
+        <v>15</v>
+      </c>
+      <c r="F572" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="573" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A573" t="s">
+        <v>8</v>
+      </c>
+      <c r="B573" t="s">
+        <v>13</v>
+      </c>
+      <c r="C573" t="s">
+        <v>6</v>
+      </c>
+      <c r="D573">
+        <v>1.89</v>
+      </c>
+      <c r="E573" t="s">
+        <v>15</v>
+      </c>
+      <c r="F573" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="574" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A574" t="s">
+        <v>8</v>
+      </c>
+      <c r="B574" t="s">
+        <v>13</v>
+      </c>
+      <c r="C574" t="s">
+        <v>6</v>
+      </c>
+      <c r="D574">
+        <v>2.89</v>
+      </c>
+      <c r="E574" t="s">
+        <v>15</v>
+      </c>
+      <c r="F574" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="575" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A575" t="s">
+        <v>8</v>
+      </c>
+      <c r="B575" t="s">
+        <v>13</v>
+      </c>
+      <c r="C575" t="s">
+        <v>6</v>
+      </c>
+      <c r="D575">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E575" t="s">
+        <v>15</v>
+      </c>
+      <c r="F575" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="576" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A576" t="s">
+        <v>8</v>
+      </c>
+      <c r="B576" t="s">
+        <v>13</v>
+      </c>
+      <c r="C576" t="s">
+        <v>6</v>
+      </c>
+      <c r="D576">
+        <v>1.96</v>
+      </c>
+      <c r="E576" t="s">
+        <v>15</v>
+      </c>
+      <c r="F576" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="577" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A577" t="s">
+        <v>8</v>
+      </c>
+      <c r="B577" t="s">
+        <v>13</v>
+      </c>
+      <c r="C577" t="s">
+        <v>6</v>
+      </c>
+      <c r="D577">
+        <v>5.51</v>
+      </c>
+      <c r="E577" t="s">
+        <v>15</v>
+      </c>
+      <c r="F577" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="578" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A578" t="s">
+        <v>8</v>
+      </c>
+      <c r="B578" t="s">
+        <v>13</v>
+      </c>
+      <c r="C578" t="s">
+        <v>6</v>
+      </c>
+      <c r="D578">
+        <v>3.31</v>
+      </c>
+      <c r="E578" t="s">
+        <v>15</v>
+      </c>
+      <c r="F578" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="579" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A579" t="s">
+        <v>8</v>
+      </c>
+      <c r="B579" t="s">
+        <v>13</v>
+      </c>
+      <c r="C579" t="s">
+        <v>6</v>
+      </c>
+      <c r="D579">
+        <v>2.98</v>
+      </c>
+      <c r="E579" t="s">
+        <v>15</v>
+      </c>
+      <c r="F579" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="580" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A580" t="s">
+        <v>8</v>
+      </c>
+      <c r="B580" t="s">
+        <v>13</v>
+      </c>
+      <c r="C580" t="s">
+        <v>6</v>
+      </c>
+      <c r="D580">
+        <v>2.84</v>
+      </c>
+      <c r="E580" t="s">
+        <v>15</v>
+      </c>
+      <c r="F580" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="581" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A581" t="s">
+        <v>8</v>
+      </c>
+      <c r="B581" t="s">
+        <v>13</v>
+      </c>
+      <c r="C581" t="s">
+        <v>6</v>
+      </c>
+      <c r="D581">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="E581" t="s">
+        <v>15</v>
+      </c>
+      <c r="F581" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="582" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A582" t="s">
+        <v>5</v>
+      </c>
+      <c r="B582" t="s">
+        <v>13</v>
+      </c>
+      <c r="C582" t="s">
+        <v>6</v>
+      </c>
+      <c r="D582">
+        <v>4.18</v>
+      </c>
+      <c r="E582" t="s">
+        <v>15</v>
+      </c>
+      <c r="F582" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="583" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A583" t="s">
+        <v>5</v>
+      </c>
+      <c r="B583" t="s">
+        <v>13</v>
+      </c>
+      <c r="C583" t="s">
+        <v>6</v>
+      </c>
+      <c r="D583">
+        <v>3.58</v>
+      </c>
+      <c r="E583" t="s">
+        <v>15</v>
+      </c>
+      <c r="F583" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="584" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A584" t="s">
+        <v>5</v>
+      </c>
+      <c r="B584" t="s">
+        <v>13</v>
+      </c>
+      <c r="C584" t="s">
+        <v>6</v>
+      </c>
+      <c r="D584">
+        <v>16.48</v>
+      </c>
+      <c r="E584" t="s">
+        <v>15</v>
+      </c>
+      <c r="F584" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="585" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A585" t="s">
+        <v>5</v>
+      </c>
+      <c r="B585" t="s">
+        <v>13</v>
+      </c>
+      <c r="C585" t="s">
+        <v>6</v>
+      </c>
+      <c r="D585">
+        <v>15.06</v>
+      </c>
+      <c r="E585" t="s">
+        <v>15</v>
+      </c>
+      <c r="F585" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="586" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A586" t="s">
+        <v>5</v>
+      </c>
+      <c r="B586" t="s">
+        <v>13</v>
+      </c>
+      <c r="C586" t="s">
+        <v>6</v>
+      </c>
+      <c r="D586">
+        <v>7.68</v>
+      </c>
+      <c r="E586" t="s">
+        <v>15</v>
+      </c>
+      <c r="F586" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="587" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A587" t="s">
+        <v>5</v>
+      </c>
+      <c r="B587" t="s">
+        <v>13</v>
+      </c>
+      <c r="C587" t="s">
+        <v>6</v>
+      </c>
+      <c r="D587">
+        <v>7.99</v>
+      </c>
+      <c r="E587" t="s">
+        <v>15</v>
+      </c>
+      <c r="F587" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="588" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A588" t="s">
+        <v>5</v>
+      </c>
+      <c r="B588" t="s">
+        <v>13</v>
+      </c>
+      <c r="C588" t="s">
+        <v>6</v>
+      </c>
+      <c r="D588">
+        <v>3.06</v>
+      </c>
+      <c r="E588" t="s">
+        <v>15</v>
+      </c>
+      <c r="F588" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="589" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A589" t="s">
+        <v>5</v>
+      </c>
+      <c r="B589" t="s">
+        <v>13</v>
+      </c>
+      <c r="C589" t="s">
+        <v>6</v>
+      </c>
+      <c r="D589">
+        <v>11.53</v>
+      </c>
+      <c r="E589" t="s">
+        <v>15</v>
+      </c>
+      <c r="F589" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="590" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A590" t="s">
+        <v>5</v>
+      </c>
+      <c r="B590" t="s">
+        <v>13</v>
+      </c>
+      <c r="C590" t="s">
+        <v>6</v>
+      </c>
+      <c r="D590">
+        <v>8.23</v>
+      </c>
+      <c r="E590" t="s">
+        <v>15</v>
+      </c>
+      <c r="F590" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="591" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A591" t="s">
+        <v>5</v>
+      </c>
+      <c r="B591" t="s">
+        <v>13</v>
+      </c>
+      <c r="C591" t="s">
+        <v>6</v>
+      </c>
+      <c r="D591">
+        <v>11.88</v>
+      </c>
+      <c r="E591" t="s">
+        <v>15</v>
+      </c>
+      <c r="F591" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="592" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A592" t="s">
+        <v>5</v>
+      </c>
+      <c r="B592" t="s">
+        <v>13</v>
+      </c>
+      <c r="C592" t="s">
+        <v>6</v>
+      </c>
+      <c r="D592">
+        <v>7.09</v>
+      </c>
+      <c r="E592" t="s">
+        <v>15</v>
+      </c>
+      <c r="F592" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="593" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A593" t="s">
+        <v>5</v>
+      </c>
+      <c r="B593" t="s">
+        <v>13</v>
+      </c>
+      <c r="C593" t="s">
+        <v>6</v>
+      </c>
+      <c r="D593">
+        <v>6.41</v>
+      </c>
+      <c r="E593" t="s">
+        <v>15</v>
+      </c>
+      <c r="F593" s="1">
+        <v>44656</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
2 new assays added
</commit_message>
<xml_diff>
--- a/data/octanol_30pct_avoidance_ALLDATA.xlsx
+++ b/data/octanol_30pct_avoidance_ALLDATA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tiabrown/Documents/git/cest-2.1-Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4888D707-4E76-FE4C-AA46-A35BC8679CFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE21B77-9CFD-F548-8CAA-2DE02C1B3378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="500" windowWidth="27720" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -980,8 +980,8 @@
   <dimension ref="A1:I2138"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2108" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2110" sqref="C2110"/>
+      <pane ySplit="1" topLeftCell="A2037" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D2047" sqref="D2047:D2069"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>